<commit_message>
added communication folder to the prep folder to organize talking points and communication matterials
</commit_message>
<xml_diff>
--- a/region2017/reports/documents/goal_scores.xlsx
+++ b/region2017/reports/documents/goal_scores.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="1180" windowWidth="28160" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="6820" yWindow="1080" windowWidth="28160" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="summary" sheetId="1" r:id="rId1"/>
+    <sheet name="LE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Region</t>
   </si>
@@ -93,16 +94,38 @@
   </si>
   <si>
     <t>Kaui &amp; Niʻihau</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Trend</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Kauai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,17 +160,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +452,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -445,21 +469,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2"/>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="3" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -530,4 +554,89 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>88.62</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>94.89</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>75.430000000000007</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>76.11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
AO updated using shoreline access weights based on roads, slope, and MPA or no fishing areas
</commit_message>
<xml_diff>
--- a/region2017/reports/documents/goal_scores.xlsx
+++ b/region2017/reports/documents/goal_scores.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="1080" windowWidth="28160" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1080" windowWidth="28160" windowHeight="16820" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
     <sheet name="LE" sheetId="2" r:id="rId2"/>
+    <sheet name="AO" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>Region</t>
   </si>
@@ -109,6 +110,18 @@
   </si>
   <si>
     <t>Kauai</t>
+  </si>
+  <si>
+    <t>Ocean Jobs</t>
+  </si>
+  <si>
+    <t>Kauai &amp; Niʻihau</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Resource</t>
   </si>
 </sst>
 </file>
@@ -165,13 +178,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -465,31 +478,31 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="3"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2"/>
+      <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
@@ -558,82 +571,231 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2">
+        <v>88.62</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>94.89</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2">
+        <v>75.430000000000007</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>76.11</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>13576</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>25423</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>59163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15">
+        <v>5264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="4">
-        <v>88.62</v>
-      </c>
-      <c r="D2" s="4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>0.64</v>
+      </c>
+      <c r="C2">
+        <v>0.66</v>
+      </c>
+      <c r="D2">
+        <v>0.65</v>
+      </c>
+      <c r="E2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C3">
+        <v>0.66</v>
+      </c>
+      <c r="D3">
+        <v>0.61</v>
+      </c>
+      <c r="E3">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0.68</v>
+      </c>
+      <c r="C4">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4">
-        <v>94.89</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4">
-        <v>75.430000000000007</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4">
-        <v>76.11</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.55000000000000004</v>
+      <c r="D4">
+        <v>0.61</v>
+      </c>
+      <c r="E4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C5">
+        <v>0.72</v>
+      </c>
+      <c r="D5">
+        <v>0.64</v>
+      </c>
+      <c r="E5">
+        <v>0.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added goal_score_tables.R to documentation to transform scores.csv into format for importing into goal tables in documentation and reports
</commit_message>
<xml_diff>
--- a/region2017/reports/documents/goal_scores.xlsx
+++ b/region2017/reports/documents/goal_scores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1640" windowWidth="26860" windowHeight="16820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="1100" windowWidth="26860" windowHeight="16820" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="AO" sheetId="3" r:id="rId5"/>
     <sheet name="ST" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="46">
   <si>
     <t>Region</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure </t>
+  </si>
+  <si>
+    <t>Resilience</t>
+  </si>
+  <si>
+    <t>Future</t>
   </si>
 </sst>
 </file>
@@ -305,16 +314,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -344,6 +344,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -658,37 +667,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="24"/>
+      <c r="H1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="14" t="s">
+      <c r="J1" s="25"/>
+      <c r="K1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="13"/>
+      <c r="M1" s="24"/>
       <c r="O1" t="s">
         <v>31</v>
       </c>
@@ -700,218 +709,218 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="16" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16" t="s">
+      <c r="K2" s="13"/>
+      <c r="L2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="13" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13">
         <v>87</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="13">
         <v>53</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="13">
         <v>45</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <v>64</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16">
+      <c r="G3" s="13"/>
+      <c r="H3" s="13">
         <v>59</v>
       </c>
-      <c r="I3" s="16">
+      <c r="I3" s="13">
         <v>59</v>
       </c>
-      <c r="J3" s="16">
+      <c r="J3" s="13">
         <v>78</v>
       </c>
-      <c r="K3" s="16">
+      <c r="K3" s="13">
         <v>50</v>
       </c>
-      <c r="L3" s="16">
+      <c r="L3" s="13">
         <v>92</v>
       </c>
-      <c r="M3" s="16">
+      <c r="M3" s="13">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13">
         <v>89</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="13">
         <v>73</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="13">
         <v>49</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="13">
         <v>92</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16">
+      <c r="G4" s="13"/>
+      <c r="H4" s="13">
         <v>59</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="13">
         <v>51</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="13">
         <v>80</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="13">
         <v>46</v>
       </c>
-      <c r="L4" s="16">
+      <c r="L4" s="13">
         <v>94</v>
       </c>
-      <c r="M4" s="16">
+      <c r="M4" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13">
         <v>83</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>41</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>42</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="13">
         <v>81</v>
       </c>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
         <v>72</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="13">
         <v>68</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="13">
         <v>78</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="13">
         <v>54</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="13">
         <v>97</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="13">
         <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16">
+      <c r="B6" s="13"/>
+      <c r="C6" s="13">
         <v>85</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="13">
         <v>34</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="13">
         <v>41</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="13">
         <v>46</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13">
         <v>51</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="13">
         <v>46</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="13">
         <v>72</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="13">
         <v>42</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="13">
         <v>88</v>
       </c>
-      <c r="M6" s="16">
+      <c r="M6" s="13">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13">
         <v>91</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="13">
         <v>64</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="13">
         <v>46</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="13">
         <v>36</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13">
         <v>54</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="13">
         <v>71</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="13">
         <v>81</v>
       </c>
-      <c r="K7" s="16">
+      <c r="K7" s="13">
         <v>57</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="13">
         <v>84</v>
       </c>
-      <c r="M7" s="16">
+      <c r="M7" s="13">
         <v>100</v>
       </c>
     </row>
@@ -932,7 +941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -944,65 +953,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="18">
         <v>2694641</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="19">
         <v>0.81</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="18">
         <v>428181</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="19">
         <v>0.88</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="18">
         <v>583030</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="21">
         <v>30230053</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="22">
         <v>0.8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="17">
         <f>SUM(B2:B5)</f>
         <v>33935905</v>
       </c>
@@ -1026,19 +1035,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,8 +1061,20 @@
       <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -1060,13 +1082,19 @@
         <v>15</v>
       </c>
       <c r="C2" s="1">
-        <v>88.62</v>
+        <v>94</v>
       </c>
       <c r="D2" s="1">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.77</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1074,13 +1102,19 @@
         <v>15</v>
       </c>
       <c r="C3" s="1">
-        <v>94.89</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>-0.22</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1088,13 +1122,19 @@
         <v>15</v>
       </c>
       <c r="C4" s="1">
-        <v>75.430000000000007</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1">
-        <v>0.51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.76</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1102,18 +1142,24 @@
         <v>15</v>
       </c>
       <c r="C5" s="1">
-        <v>76.11</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>0.77</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2013</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1121,7 +1167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1175,7 @@
         <v>13576</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1137,7 +1183,7 @@
         <v>25423</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1145,7 +1191,7 @@
         <v>59163</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1160,15 +1206,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1185,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -1202,7 +1248,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -1219,7 +1265,7 @@
         <v>-0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -1236,7 +1282,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1251,6 +1297,136 @@
       </c>
       <c r="E5" s="3">
         <v>0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>82</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="2">
+        <v>24.9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>83.6</v>
+      </c>
+      <c r="G9" s="2">
+        <v>98</v>
+      </c>
+      <c r="H9" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>79</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-0.01</v>
+      </c>
+      <c r="E10" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>77.3</v>
+      </c>
+      <c r="G10" s="2">
+        <v>89</v>
+      </c>
+      <c r="H10" s="2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="E11" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>67.5</v>
+      </c>
+      <c r="G11" s="2">
+        <v>70</v>
+      </c>
+      <c r="H11" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>82</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="E12" s="3">
+        <v>29.9</v>
+      </c>
+      <c r="F12" s="3">
+        <v>54.8</v>
+      </c>
+      <c r="G12" s="3">
+        <v>90</v>
+      </c>
+      <c r="H12" s="3">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1260,10 +1436,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1274,7 +1450,7 @@
     <col min="5" max="5" width="7.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1467,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>17</v>
       </c>
@@ -1306,7 +1482,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
@@ -1323,7 +1499,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -1340,7 +1516,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>20</v>
       </c>
@@ -1357,7 +1533,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
@@ -1372,6 +1548,136 @@
       </c>
       <c r="E6" s="11">
         <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2">
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="E9" s="2">
+        <v>24.9</v>
+      </c>
+      <c r="F9" s="2">
+        <v>55.4</v>
+      </c>
+      <c r="G9" s="2">
+        <v>57</v>
+      </c>
+      <c r="H9" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>75</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-0.25</v>
+      </c>
+      <c r="E10" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>56.8</v>
+      </c>
+      <c r="G10" s="2">
+        <v>70</v>
+      </c>
+      <c r="H10" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2">
+        <v>-0.4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>39.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>52.7</v>
+      </c>
+      <c r="G11" s="2">
+        <v>46</v>
+      </c>
+      <c r="H11" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="E12" s="3">
+        <v>29.9</v>
+      </c>
+      <c r="F12" s="3">
+        <v>55.1</v>
+      </c>
+      <c r="G12" s="3">
+        <v>49</v>
+      </c>
+      <c r="H12" s="3">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>